<commit_message>
Remove pulit18's waist-hip-ratio as trait
</commit_message>
<xml_diff>
--- a/1_data/gwas_summstats/hcm_related_traits_summary.xlsx
+++ b/1_data/gwas_summstats/hcm_related_traits_summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jon Chan\Documents\R Projects\Watkins_Offline\MultiPheno_HCM_MR\1_data\gwas_summstats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53914D83-EBB2-4A14-83CA-00D1B4BA308B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B67C31B-F858-4DB0-B18E-AC5D83F07681}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="17385" xr2:uid="{73FD91AA-0239-4790-95FD-809D24710730}"/>
+    <workbookView xWindow="2670" yWindow="2190" windowWidth="21600" windowHeight="12645" xr2:uid="{73FD91AA-0239-4790-95FD-809D24710730}"/>
   </bookViews>
   <sheets>
     <sheet name="GWAS Summstats" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="102">
   <si>
     <t>TRAIT GROUP</t>
   </si>
@@ -173,15 +173,9 @@
     <t>BMI-adjusted waist-hip ratio</t>
   </si>
   <si>
-    <t>https://www.ebi.ac.uk/gwas/studies/GCST008994</t>
-  </si>
-  <si>
     <t>Pulit et al, 2018</t>
   </si>
   <si>
-    <t>European ancestry</t>
-  </si>
-  <si>
     <t>https://academic.oup.com/hmg/article/28/1/166/5098227?login=true</t>
   </si>
   <si>
@@ -227,9 +221,6 @@
     <t>Miyazawa et al, 2023</t>
   </si>
   <si>
-    <t>https://www.ebi.ac.uk/gwas/studies/GCST90204201</t>
-  </si>
-  <si>
     <t>https://www.nature.com/articles/s41588-022-01284-9</t>
   </si>
   <si>
@@ -329,83 +320,35 @@
     <t>Tadros et al, 2025</t>
   </si>
   <si>
-    <t>Absolute .tsv.gz Path</t>
-  </si>
-  <si>
-    <t>/well/PROCARDIS/jchan/misc/gwas_summstats/ECG/rr_interval/choi21/TOPMed_freeze6_common_singlevariant_RR.tsv.gz</t>
-  </si>
-  <si>
-    <t>/well/PROCARDIS/jchan/misc/gwas_summstats/ECG/gzip qtc_interval/choi21/TOPMed_freeze6_common_singlevariant_QTc.tsv.gz</t>
-  </si>
-  <si>
-    <t>/well/PROCARDIS/jchan/misc/gwas_summstats/ECG/choi21/TOPMed_freeze6_common_singlevariant_QRS.tsv.gz</t>
-  </si>
-  <si>
-    <t>/well/PROCARDIS/jchan/misc/gwas_summstats/ECG/pwave_duration/TOPMed_freeze6_common_singlevariant_Pdur.tsv.gz</t>
-  </si>
-  <si>
-    <t>/well/PROCARDIS/jchan/misc/gwas_summstats/ECG/pr_interval/ntalla20/PR_1000g_GWAS_EUR.tsv.gz</t>
-  </si>
-  <si>
-    <t>/well/PROCARDIS/jchan/misc/gwas_summstats/ECG/qt_interval/hoffmann22/GCST90165290_buildGRCh37.tsv.gz</t>
-  </si>
-  <si>
-    <t>/well/PROCARDIS/jchan/misc/gwas_summstats/CMR/t1_time/nauffal24/native_myocardial_t1_time_summstats.tsv.gz</t>
-  </si>
-  <si>
-    <t>/well/PROCARDIS/jchan/misc/gwas_summstats/CRF/alcohol/liu19/DrinksPerWeek.tsv.gz</t>
-  </si>
-  <si>
-    <t>/well/PROCARDIS/jchan/misc/gwas_summstats/CRF/smoking_initiation/liu19/SmokingInitiation.tsv.gz</t>
-  </si>
-  <si>
-    <t>/well/PROCARDIS/jchan/misc/gwas_summstats/CRF/af/miyazawa23/GCST90204201_buildGRCh37.tsv.gz</t>
-  </si>
-  <si>
-    <t>/well/PROCARDIS/jchan/misc/gwas_summstats/CRF/bmi/sidorenko24/GCST90446645.tsv.gz</t>
-  </si>
-  <si>
-    <t>/well/PROCARDIS/jchan/misc/gwas_summstats/CRF/t2d/sakaue21/GCST90018926_buildGRCh37.tsv.gz</t>
-  </si>
-  <si>
-    <t>/well/PROCARDIS/jchan/misc/gwas_summstats/HF/levin22/GCST90162626_buildGRCh37.tsv.gz</t>
-  </si>
-  <si>
-    <t>/well/PROCARDIS/jchan/misc/gwas_summstats/CMR/maxRAAi/pirrucello22/invnorm_ramax_area_indexed.tsv.gz</t>
-  </si>
-  <si>
-    <t>/well/PROCARDIS/jchan/misc/gwas_summstats/CMR/radial_dsr/thanaj22/GCST90019014_buildGRCh37.tsv.gz</t>
-  </si>
-  <si>
-    <t>/well/PROCARDIS/jchan/misc/gwas_summstats/CMR/minRAAi/pirrucello22/invnorm_ramin_area_indexed.tsv.gz</t>
-  </si>
-  <si>
-    <t>/well/PROCARDIS/jchan/misc/gwas_summstats/CMR/rvsvi/pirrucello22/invnorm_RVSV_indexed.tsv.gz</t>
-  </si>
-  <si>
-    <t>/well/PROCARDIS/jchan/misc/gwas_summstats/CMR/rvef/pirrucello22/invnorm_RVEF.tsv.gz</t>
-  </si>
-  <si>
-    <t>/well/PROCARDIS/jchan/misc/gwas_summstats/CMR/maxLAVi/thanaj22/GCST90019012_buildGRCh37.tsv.gz</t>
-  </si>
-  <si>
-    <t>/well/PROCARDIS/jchan/misc/gwas_summstats/CMR/RAfrac_change/pirrucello22/invnorm_rafac.tsv.gz</t>
-  </si>
-  <si>
-    <t>/well/PROCARDIS/jchan/misc/gwas_summstats/CMR/rvesvi/pirrucello22/invnorm_RVESV_indexed.tsv.gz</t>
-  </si>
-  <si>
-    <t>/well/PROCARDIS/jchan/misc/gwas_summstats/CMR/rvedvi/pirrucello22/invnorm_RVEDV_indexed.tsv.gz</t>
-  </si>
-  <si>
-    <t>/well/PROCARDIS/jchan/misc/gwas_summstats/HCM/Tadros24/nonMTAG/hcm.fix.2024.format.tsv.gz</t>
+    <t>C-reactive Protein</t>
+  </si>
+  <si>
+    <t>https://www.nature.com/articles/s41467-022-34688-6</t>
+  </si>
+  <si>
+    <t>Koskeridis  et al, 2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.ebi.ac.uk/gwas/studies/GCST90179146 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.ebi.ac.uk/gwas/studies/GCST90204201 </t>
+  </si>
+  <si>
+    <t>https://www.ebi.ac.uk/gwas/efotraits/EFO_0007788</t>
+  </si>
+  <si>
+    <t>European ancestry females</t>
+  </si>
+  <si>
+    <t>ITALICS MEANS IGNORED FOR NOW</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -456,6 +399,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -496,10 +448,8 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -835,10 +785,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98643D4D-D81F-488C-AE56-A70D10E094CB}">
-  <dimension ref="A1:K34"/>
+  <dimension ref="A1:P35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="P1" sqref="P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -848,11 +798,10 @@
     <col min="3" max="4" width="10.7109375" style="1" customWidth="1"/>
     <col min="5" max="5" width="32.42578125" style="1" customWidth="1"/>
     <col min="6" max="7" width="10.7109375" customWidth="1"/>
-    <col min="10" max="10" width="27.140625" style="4" customWidth="1"/>
-    <col min="11" max="11" width="9.140625" style="4"/>
+    <col min="10" max="10" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -875,13 +824,13 @@
         <v>12</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+      <c r="P1" s="9" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -889,25 +838,22 @@
       <c r="E2" s="3"/>
       <c r="G2" s="3"/>
     </row>
-    <row r="3" spans="1:11" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
-      <c r="B3" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>96</v>
+      <c r="B3" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>93</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="G3" s="3"/>
       <c r="J3" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -923,277 +869,249 @@
       <c r="E5" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="5" t="s">
         <v>43</v>
       </c>
       <c r="G5" t="s">
         <v>40</v>
       </c>
-      <c r="J5" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="K5" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="B6" s="1" t="s">
+      <c r="J5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="B6" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6" s="7">
+        <v>379501</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="G6" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="D6" s="1">
-        <v>379501</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F6" t="s">
-        <v>45</v>
-      </c>
-      <c r="G6" t="s">
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="9" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="B7" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="K6" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="B7" s="1" t="s">
-        <v>50</v>
-      </c>
       <c r="C7" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D7" s="1">
         <f>490089+177415</f>
         <v>667504</v>
       </c>
       <c r="E7" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="G7" t="s">
+        <v>51</v>
+      </c>
+      <c r="J7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+      <c r="B8" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F7" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="G7" t="s">
+      <c r="C8" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="J7" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="K7" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="B8" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>55</v>
       </c>
       <c r="D8" s="1">
         <v>1232091</v>
       </c>
       <c r="E8" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="G8" t="s">
+        <v>56</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="F8" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="G8" t="s">
-        <v>58</v>
-      </c>
-      <c r="J8" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="K8" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="B9" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="C9" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D9" s="1">
         <v>941280</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="F9" t="s">
+        <v>55</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="G9" t="s">
+        <v>56</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="B10" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D10" s="1">
+        <v>575531</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="G10" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="G9" t="s">
-        <v>58</v>
-      </c>
-      <c r="J9" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="K9" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="B10" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D10" s="1">
+      <c r="D11" s="1">
         <f>1244730+1094458</f>
         <v>2339188</v>
       </c>
-      <c r="E10" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F10" t="s">
-        <v>63</v>
-      </c>
-      <c r="G10" t="s">
-        <v>64</v>
-      </c>
-      <c r="J10" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="K10" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="7" t="s">
+      <c r="E11" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="G11" t="s">
+        <v>61</v>
+      </c>
+      <c r="J11" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="G12" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+    </row>
+    <row r="13" spans="1:16" s="1" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="8" t="s">
+      <c r="D13" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="G13" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="G11" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="10"/>
-    </row>
-    <row r="12" spans="1:11" s="1" customFormat="1" ht="135" x14ac:dyDescent="0.25">
-      <c r="B12" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="J12" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="K12" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+      <c r="J13" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B15" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C15" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D14" s="1">
+      <c r="D15" s="1">
         <v>76995</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E15" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F15" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G14" t="s">
+      <c r="G15" t="s">
         <v>13</v>
       </c>
-      <c r="J14" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="K14" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="B15" s="1" t="s">
+      <c r="J15" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="B16" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C16" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D15" s="1">
+      <c r="D16" s="1">
         <v>271570</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="E16" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F16" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="G15" t="s">
+      <c r="G16" t="s">
         <v>17</v>
       </c>
-      <c r="J15" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="K15" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="7"/>
-      <c r="B16" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D16" s="7">
-        <v>44456</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F16" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="G16" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="J16" s="10"/>
-      <c r="K16" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="J16" s="4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
       <c r="B17" s="7" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C17" s="7" t="s">
         <v>24</v>
@@ -1205,45 +1123,42 @@
         <v>22</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G17" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="J17" s="10"/>
-      <c r="K17" s="4" t="s">
+      <c r="J17" s="9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="B18" s="1" t="s">
+    <row r="18" spans="1:10" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" s="7"/>
+      <c r="B18" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D18" s="1">
-        <v>29000</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F18" t="s">
-        <v>38</v>
-      </c>
-      <c r="G18" t="s">
-        <v>32</v>
-      </c>
-      <c r="J18" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="K18" s="4" t="s">
+      <c r="C18" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D18" s="7">
+        <v>44456</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="J18" s="9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>34</v>
@@ -1254,22 +1169,19 @@
       <c r="E19" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F19" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="G19" t="s">
+      <c r="G19" s="5" t="s">
         <v>32</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="K19" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>34</v>
@@ -1287,202 +1199,180 @@
         <v>32</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="K20" s="4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="B21" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D21" s="1">
+        <v>29000</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F21" t="s">
+        <v>38</v>
+      </c>
+      <c r="G21" t="s">
+        <v>32</v>
+      </c>
+      <c r="J21" s="4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="7"/>
+      <c r="B22" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D22" s="7">
+        <v>29000</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="G22" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="J22" s="9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:11" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="7"/>
-      <c r="B21" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="C21" s="7" t="s">
+    <row r="23" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="B23" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D21" s="7">
+      <c r="D23" s="1">
         <v>29000</v>
       </c>
-      <c r="E21" s="7" t="s">
+      <c r="E23" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F21" s="8" t="s">
+      <c r="F23" t="s">
         <v>38</v>
       </c>
-      <c r="G21" s="8" t="s">
+      <c r="G23" t="s">
         <v>32</v>
       </c>
-      <c r="J21" s="10"/>
-      <c r="K21" s="10" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="B22" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D22" s="1">
-        <v>29000</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F22" t="s">
-        <v>38</v>
-      </c>
-      <c r="G22" t="s">
-        <v>32</v>
-      </c>
-      <c r="J22" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="K22" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
+      <c r="J23" s="4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B25" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C25" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D24" s="1">
+      <c r="D25" s="1">
         <v>43881</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F24" t="s">
-        <v>30</v>
-      </c>
-      <c r="G24" t="s">
-        <v>27</v>
-      </c>
-      <c r="J24" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="K24" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="B25" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D25" s="1">
-        <v>39559</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F25" t="s">
-        <v>69</v>
+      <c r="F25" s="5" t="s">
+        <v>30</v>
       </c>
       <c r="G25" t="s">
-        <v>66</v>
+        <v>27</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="K25" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D26" s="1">
-        <v>39560</v>
+        <v>39559</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F26" t="s">
-        <v>70</v>
+      <c r="F26" s="5" t="s">
+        <v>66</v>
       </c>
       <c r="G26" t="s">
-        <v>66</v>
-      </c>
-      <c r="J26" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="K26" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+      <c r="J26" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D27" s="1">
-        <v>39561</v>
+        <v>39560</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F27" t="s">
-        <v>68</v>
+      <c r="F27" s="5" t="s">
+        <v>67</v>
       </c>
       <c r="G27" t="s">
-        <v>66</v>
-      </c>
-      <c r="J27" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="K27" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+      <c r="J27" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="D28" s="1">
-        <v>40000</v>
+        <v>39561</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F28" t="s">
-        <v>75</v>
+      <c r="F28" s="5" t="s">
+        <v>65</v>
       </c>
       <c r="G28" t="s">
+        <v>63</v>
+      </c>
+      <c r="J28" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="B29" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="J28" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="K28" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="B29" s="1" t="s">
-        <v>78</v>
-      </c>
       <c r="C29" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D29" s="1">
         <v>40000</v>
@@ -1490,25 +1380,22 @@
       <c r="E29" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F29" t="s">
+      <c r="F29" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="G29" t="s">
+        <v>71</v>
+      </c>
+      <c r="J29" s="4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="B30" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="G29" t="s">
-        <v>74</v>
-      </c>
-      <c r="J29" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="K29" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="B30" s="1" t="s">
-        <v>79</v>
-      </c>
       <c r="C30" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D30" s="1">
         <v>40000</v>
@@ -1517,24 +1404,21 @@
         <v>26</v>
       </c>
       <c r="F30" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="G30" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="J30" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="K30" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D31" s="1">
         <v>40000</v>
@@ -1543,24 +1427,21 @@
         <v>26</v>
       </c>
       <c r="F31" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="G31" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="J31" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="K31" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B32" s="1" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D32" s="1">
         <v>40000</v>
@@ -1569,24 +1450,21 @@
         <v>26</v>
       </c>
       <c r="F32" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="G32" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="J32" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="K32" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="33" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="33" spans="2:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B33" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D33" s="1">
         <v>40000</v>
@@ -1595,24 +1473,21 @@
         <v>26</v>
       </c>
       <c r="F33" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="G33" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="K33" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="34" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="34" spans="2:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B34" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D34" s="1">
         <v>40000</v>
@@ -1621,23 +1496,58 @@
         <v>26</v>
       </c>
       <c r="F34" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="G34" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="J34" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="K34" s="4" t="s">
-        <v>3</v>
+        <v>91</v>
+      </c>
+    </row>
+    <row r="35" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="B35" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D35" s="1">
+        <v>40000</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F35" t="s">
+        <v>72</v>
+      </c>
+      <c r="G35" t="s">
+        <v>71</v>
+      </c>
+      <c r="J35" s="4" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F8" r:id="rId1" xr:uid="{ECF4F655-E178-4EE0-89D7-734F17D2F16A}"/>
     <hyperlink ref="F7" r:id="rId2" xr:uid="{1273BF52-00A0-4A9B-9D20-9D822A3E0579}"/>
+    <hyperlink ref="G19" r:id="rId3" xr:uid="{C9981D4E-A240-45B0-B8B5-79F8E1938D29}"/>
+    <hyperlink ref="F19" r:id="rId4" xr:uid="{93E1FBD9-0952-41E8-98C7-20CFAD07CAF1}"/>
+    <hyperlink ref="F25" r:id="rId5" xr:uid="{348392FE-469C-4368-AF97-0DFDFDE1BBC2}"/>
+    <hyperlink ref="F29" r:id="rId6" xr:uid="{5E4F1FBC-90EA-4C55-BF82-59E32CDDC7B1}"/>
+    <hyperlink ref="F5" r:id="rId7" xr:uid="{C2A4BD86-1C88-41DF-AF3B-FDF4185041FA}"/>
+    <hyperlink ref="F6" r:id="rId8" xr:uid="{946F0F63-1BAB-498F-A4B3-10A5E0D4B596}"/>
+    <hyperlink ref="F9" r:id="rId9" xr:uid="{028A7295-1D4D-440C-ACEC-AF44F0910DFD}"/>
+    <hyperlink ref="F10" r:id="rId10" xr:uid="{6472D517-A065-4D22-9800-CA201F182F8B}"/>
+    <hyperlink ref="F11" r:id="rId11" xr:uid="{61F7C871-3E8A-4413-B912-F298F684E6E2}"/>
+    <hyperlink ref="F15" r:id="rId12" xr:uid="{B3E8E859-E9CA-4D4C-ABBC-D2D2ACD33977}"/>
+    <hyperlink ref="F16" r:id="rId13" xr:uid="{B3AA269E-BB22-47F9-B230-CD37F742A4BD}"/>
+    <hyperlink ref="F26" r:id="rId14" xr:uid="{5DBE38BD-976C-4E7B-9259-8CBF010AB9F2}"/>
+    <hyperlink ref="F27" r:id="rId15" xr:uid="{821F5878-37F7-4D33-82CB-063EC715B57D}"/>
+    <hyperlink ref="F28" r:id="rId16" xr:uid="{87E24D2C-01A7-459A-AA07-0E9F5D9BC565}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId17"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Switch to using Loeb2024 for GWAS of eGFR
</commit_message>
<xml_diff>
--- a/1_data/gwas_summstats/hcm_related_traits_summary.xlsx
+++ b/1_data/gwas_summstats/hcm_related_traits_summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jon Chan\Documents\R Projects\Watkins_Offline\MultiPheno_HCM_MR\1_data\gwas_summstats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE5CAC27-A958-49EB-B8ED-25FDB07DA994}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{861E16F9-A430-4BC7-80A4-237CCBB74362}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{73FD91AA-0239-4790-95FD-809D24710730}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="12645" xr2:uid="{73FD91AA-0239-4790-95FD-809D24710730}"/>
   </bookViews>
   <sheets>
     <sheet name="GWAS Summstats" sheetId="1" r:id="rId1"/>
@@ -371,22 +371,22 @@
     <t>https://www.nature.com/articles/s41588-024-01714-w</t>
   </si>
   <si>
-    <t>Estimated Glomerular Filtration Rate (creatinine)</t>
-  </si>
-  <si>
-    <t>Liu et al, 2022</t>
-  </si>
-  <si>
-    <t>https://www.nature.com/articles/s41588-022-01097-w</t>
-  </si>
-  <si>
-    <t>https://www.ebi.ac.uk/gwas/studies/GCST90100220</t>
-  </si>
-  <si>
-    <t>1,205,871 European ancestry individuals, 168,300 East Asian ancestry individuals, 63,553 African ancestry individuals, 23,509 Hispanic or Latin American individuals, 22,103 African American individuals, 21,791 Central Asian or South Asian ancestry individuals, 1,502 Middle Eastern ancestry individuals, 939 other admixed ancestry individuals, 602 Native American ancestry individuals, 150 Asian ancestry individuals, 339 individuals</t>
-  </si>
-  <si>
     <t>Supp. Table 6</t>
+  </si>
+  <si>
+    <t>Estimated Glomerular Filtration Rate (creatinine; cystatin C)</t>
+  </si>
+  <si>
+    <t>Loeb et al, 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> European ancestry individuals</t>
+  </si>
+  <si>
+    <t>https://www.ebi.ac.uk/gwas/studies/GCST90428446</t>
+  </si>
+  <si>
+    <t>https://www.nature.com/articles/s41588-024-01904-6</t>
   </si>
 </sst>
 </file>
@@ -489,7 +489,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -514,6 +514,9 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -851,8 +854,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98643D4D-D81F-488C-AE56-A70D10E094CB}">
   <dimension ref="A1:P38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1041,21 +1044,24 @@
         <v>56</v>
       </c>
     </row>
-    <row r="11" spans="1:16" ht="225" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" ht="75" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
+      </c>
+      <c r="D11" s="14">
+        <v>406504</v>
       </c>
       <c r="E11" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F11" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="F11" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="G11" t="s">
-        <v>113</v>
+      <c r="G11" s="5" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="12" spans="1:16" ht="30" x14ac:dyDescent="0.25">
@@ -1263,7 +1269,7 @@
         <v>32</v>
       </c>
       <c r="J22" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -1286,7 +1292,7 @@
         <v>32</v>
       </c>
       <c r="J23" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -1309,7 +1315,7 @@
         <v>32</v>
       </c>
       <c r="J24" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="25" spans="1:10" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -1353,7 +1359,7 @@
         <v>32</v>
       </c>
       <c r="J26" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -1600,8 +1606,9 @@
     <hyperlink ref="F31" r:id="rId16" xr:uid="{87E24D2C-01A7-459A-AA07-0E9F5D9BC565}"/>
     <hyperlink ref="F16" r:id="rId17" xr:uid="{134B2401-7753-4018-9860-CE334DB4FD0C}"/>
     <hyperlink ref="G33" r:id="rId18" xr:uid="{7F90313D-72F8-47C9-B2EF-7402CCA8A3AB}"/>
+    <hyperlink ref="G11" r:id="rId19" xr:uid="{C54A08BF-6753-478C-BCB8-7FBF638238F0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId19"/>
+  <pageSetup orientation="portrait" r:id="rId20"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
More stringent phenotype selection applied requiring observational association first
</commit_message>
<xml_diff>
--- a/1_data/gwas_summstats/hcm_related_traits_summary.xlsx
+++ b/1_data/gwas_summstats/hcm_related_traits_summary.xlsx
@@ -1,19 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jon Chan\Documents\R Projects\Watkins_Offline\MultiPheno_HCM_MR\1_data\gwas_summstats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDAA69F0-2854-4C0E-80D6-9604C7C76821}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F4F8DB9-FD61-427F-94A3-42C5260C10A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2295" yWindow="2295" windowWidth="21600" windowHeight="12645" xr2:uid="{73FD91AA-0239-4790-95FD-809D24710730}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{73FD91AA-0239-4790-95FD-809D24710730}"/>
   </bookViews>
   <sheets>
-    <sheet name="GWAS Summstats" sheetId="1" r:id="rId1"/>
+    <sheet name="Phenotype Selection" sheetId="3" r:id="rId1"/>
+    <sheet name="GWAS Summary Statistics" sheetId="4" r:id="rId2"/>
+    <sheet name="GWAS Summstats_Archive" sheetId="1" r:id="rId3"/>
+    <sheet name="MR IV Analysis" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="185">
   <si>
     <t>TRAIT GROUP</t>
   </si>
@@ -399,13 +402,205 @@
   </si>
   <si>
     <t>https://www.nature.com/articles/s41588-018-0171-3</t>
+  </si>
+  <si>
+    <t>LVEF</t>
+  </si>
+  <si>
+    <t>https://www.ebi.ac.uk/gwas/studies/GCST90435261</t>
+  </si>
+  <si>
+    <t>https://www.nature.com/articles/s41588-025-02087-4</t>
+  </si>
+  <si>
+    <t>IV Concerns</t>
+  </si>
+  <si>
+    <t>Run MR?</t>
+  </si>
+  <si>
+    <t>Roselli et al, 2025</t>
+  </si>
+  <si>
+    <t>Variable Group</t>
+  </si>
+  <si>
+    <t>Diseases</t>
+  </si>
+  <si>
+    <t>Clinical Risk Factors</t>
+  </si>
+  <si>
+    <t>https://www.nature.com/articles/s41588-024-02072-3</t>
+  </si>
+  <si>
+    <t>ECG Parameters</t>
+  </si>
+  <si>
+    <t>CMR Parameters</t>
+  </si>
+  <si>
+    <t>Phenotype</t>
+  </si>
+  <si>
+    <t>HCM -&gt; Phenotype?</t>
+  </si>
+  <si>
+    <t>Phenotype -&gt; HCM?</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>HCM-Associated Phenotype</t>
+  </si>
+  <si>
+    <t>Positive or Negative Association</t>
+  </si>
+  <si>
+    <t>Supporting Literature</t>
+  </si>
+  <si>
+    <t>+</t>
+  </si>
+  <si>
+    <t>Myocardial fibrosis</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>Ommen et al, 2020</t>
+  </si>
+  <si>
+    <t>Ho et al, 2010 (NEJM)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ellims et al, 2014 </t>
+  </si>
+  <si>
+    <t>Raman et al, 2018</t>
+  </si>
+  <si>
+    <t>Ho et al, 2013</t>
+  </si>
+  <si>
+    <t>DBP</t>
+  </si>
+  <si>
+    <t>Smoking</t>
+  </si>
+  <si>
+    <t>Alcohol</t>
+  </si>
+  <si>
+    <t>https://pmc.ncbi.nlm.nih.gov/articles/PMC10541040/</t>
+  </si>
+  <si>
+    <t>Zaromytidou et al, 2023</t>
+  </si>
+  <si>
+    <t>Olivotto et al, 2013</t>
+  </si>
+  <si>
+    <t>NTproBNP</t>
+  </si>
+  <si>
+    <t>Cardiac Imaging Parameters</t>
+  </si>
+  <si>
+    <t>Galectin-3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MMP1 </t>
+  </si>
+  <si>
+    <t>Plasma Proteins (UKB)</t>
+  </si>
+  <si>
+    <t>IL1RL1</t>
+  </si>
+  <si>
+    <t>Troponin I</t>
+  </si>
+  <si>
+    <t>See  Plasma Proteomics Manuscript</t>
+  </si>
+  <si>
+    <t>BNP</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Directionality of relationship unclear as some publications report fibrosis as preclinical marker + others as secondary pathological change, hence utility in evaluating by MR.</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S2666602224000107</t>
+  </si>
+  <si>
+    <t>Arabadjian et al, 2024</t>
+  </si>
+  <si>
+    <t>https://academic.oup.com/eurheartj/article/40/21/1671/5144691</t>
+  </si>
+  <si>
+    <t>Phenotypes are included if associated with HCM (i.e case-control) OR severity of HCM phenotypes</t>
+  </si>
+  <si>
+    <t>Wasserstrum et al, 2018</t>
+  </si>
+  <si>
+    <t>https://www.ahajournals.org/doi/10.1161/circulationaha.117.031912</t>
+  </si>
+  <si>
+    <t>Kamimura et al, 2018</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Qiao et al, 2023</t>
+  </si>
+  <si>
+    <t>Carasso et al, 2010</t>
+  </si>
+  <si>
+    <t>Anderssen et al, 2022</t>
+  </si>
+  <si>
+    <t>Unclear atm about the relationship between alcohol and HCM so ignored for now.</t>
+  </si>
+  <si>
+    <t>Henry et al, 2025</t>
+  </si>
+  <si>
+    <t>Positive control traits (from prior MR)</t>
+  </si>
+  <si>
+    <t>GWAS Summary Statistics Available?</t>
+  </si>
+  <si>
+    <t>Non-sustained ventricular tachycardia</t>
+  </si>
+  <si>
+    <t>Diastolic function e.g maxLAVi, diastolic strain rates</t>
+  </si>
+  <si>
+    <t>Myocardial fibrosis - native T1 time</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -479,6 +674,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -488,7 +706,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -496,12 +714,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -528,6 +755,72 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -863,11 +1156,612 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03D9F7EA-4DDA-48FD-9498-CF39562BE23A}">
+  <dimension ref="A1:H26"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18:B19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.140625" style="19" customWidth="1"/>
+    <col min="2" max="2" width="27.140625" style="16" customWidth="1"/>
+    <col min="3" max="3" width="18" style="16" customWidth="1"/>
+    <col min="4" max="4" width="36.28515625" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" style="23" customWidth="1"/>
+    <col min="6" max="6" width="52.5703125" style="29" customWidth="1"/>
+    <col min="7" max="7" width="17.140625" customWidth="1"/>
+    <col min="8" max="8" width="36.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="20" customFormat="1" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="33" t="s">
+        <v>127</v>
+      </c>
+      <c r="B1" s="33" t="s">
+        <v>138</v>
+      </c>
+      <c r="C1" s="33" t="s">
+        <v>139</v>
+      </c>
+      <c r="D1" s="33" t="s">
+        <v>140</v>
+      </c>
+      <c r="E1" s="34" t="s">
+        <v>144</v>
+      </c>
+      <c r="F1" s="33" t="s">
+        <v>143</v>
+      </c>
+      <c r="G1" s="20" t="s">
+        <v>181</v>
+      </c>
+      <c r="H1" s="20" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="25" t="s">
+        <v>128</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="D3" t="s">
+        <v>145</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="25"/>
+      <c r="B4" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="D4" t="s">
+        <v>179</v>
+      </c>
+      <c r="G4" s="16" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B5" s="35" t="s">
+        <v>182</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="D5" t="s">
+        <v>145</v>
+      </c>
+      <c r="G5" s="16" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="25" t="s">
+        <v>129</v>
+      </c>
+      <c r="B7" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="26" t="s">
+        <v>141</v>
+      </c>
+      <c r="D7" t="s">
+        <v>155</v>
+      </c>
+      <c r="G7" s="26" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="25"/>
+      <c r="B8" s="26"/>
+      <c r="C8" s="26"/>
+      <c r="D8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E8" s="23" t="s">
+        <v>153</v>
+      </c>
+      <c r="F8" s="30" t="s">
+        <v>180</v>
+      </c>
+      <c r="G8" s="26"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="25"/>
+      <c r="B9" s="16" t="s">
+        <v>150</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="D9" t="s">
+        <v>168</v>
+      </c>
+      <c r="E9" s="23" t="s">
+        <v>167</v>
+      </c>
+      <c r="F9" s="30" t="s">
+        <v>180</v>
+      </c>
+      <c r="G9" s="16" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="25"/>
+      <c r="B10" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="D10" t="s">
+        <v>171</v>
+      </c>
+      <c r="E10" s="24" t="s">
+        <v>169</v>
+      </c>
+      <c r="G10" s="16" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="25"/>
+      <c r="B11" s="16" t="s">
+        <v>151</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="D11" t="s">
+        <v>173</v>
+      </c>
+      <c r="E11" s="23" t="s">
+        <v>172</v>
+      </c>
+      <c r="G11" s="16" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="25"/>
+      <c r="B12" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="D12" t="s">
+        <v>177</v>
+      </c>
+      <c r="F12" s="32" t="s">
+        <v>178</v>
+      </c>
+      <c r="G12" s="16" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="27" t="s">
+        <v>157</v>
+      </c>
+      <c r="B14" s="26" t="s">
+        <v>142</v>
+      </c>
+      <c r="C14" s="26" t="s">
+        <v>141</v>
+      </c>
+      <c r="D14" t="s">
+        <v>146</v>
+      </c>
+      <c r="F14" s="31" t="s">
+        <v>166</v>
+      </c>
+      <c r="G14" s="26" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="27"/>
+      <c r="B15" s="26"/>
+      <c r="C15" s="26"/>
+      <c r="D15" t="s">
+        <v>149</v>
+      </c>
+      <c r="F15" s="31"/>
+      <c r="G15" s="26"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="27"/>
+      <c r="B16" s="26"/>
+      <c r="C16" s="26"/>
+      <c r="D16" t="s">
+        <v>147</v>
+      </c>
+      <c r="F16" s="31"/>
+      <c r="G16" s="26"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="27"/>
+      <c r="B17" s="26"/>
+      <c r="C17" s="26"/>
+      <c r="D17" t="s">
+        <v>148</v>
+      </c>
+      <c r="F17" s="31"/>
+      <c r="G17" s="26"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="27"/>
+      <c r="B18" s="36" t="s">
+        <v>183</v>
+      </c>
+      <c r="C18" s="26" t="s">
+        <v>165</v>
+      </c>
+      <c r="D18" t="s">
+        <v>175</v>
+      </c>
+      <c r="F18" s="32"/>
+      <c r="G18" s="16" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="27"/>
+      <c r="B19" s="36"/>
+      <c r="C19" s="26"/>
+      <c r="D19" t="s">
+        <v>176</v>
+      </c>
+      <c r="F19" s="32"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="15"/>
+      <c r="B20" s="18"/>
+      <c r="C20" s="18"/>
+      <c r="F20" s="32"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="25" t="s">
+        <v>160</v>
+      </c>
+      <c r="B21" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C21" s="26" t="s">
+        <v>141</v>
+      </c>
+      <c r="D21" s="26" t="s">
+        <v>163</v>
+      </c>
+      <c r="G21" s="16" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="25"/>
+      <c r="B22" s="16" t="s">
+        <v>164</v>
+      </c>
+      <c r="C22" s="26"/>
+      <c r="D22" s="26"/>
+      <c r="G22" s="16" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="25"/>
+      <c r="B23" s="16" t="s">
+        <v>162</v>
+      </c>
+      <c r="C23" s="26"/>
+      <c r="D23" s="26"/>
+      <c r="G23" s="16" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="25"/>
+      <c r="B24" s="16" t="s">
+        <v>159</v>
+      </c>
+      <c r="C24" s="26"/>
+      <c r="D24" s="26"/>
+      <c r="G24" s="16" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="25"/>
+      <c r="B25" s="16" t="s">
+        <v>158</v>
+      </c>
+      <c r="C25" s="26"/>
+      <c r="D25" s="26"/>
+      <c r="G25" s="16" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="25"/>
+      <c r="B26" s="16" t="s">
+        <v>161</v>
+      </c>
+      <c r="C26" s="26"/>
+      <c r="D26" s="26"/>
+      <c r="G26" s="16" t="s">
+        <v>137</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="15">
+    <mergeCell ref="G14:G17"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C14:C17"/>
+    <mergeCell ref="A14:A19"/>
+    <mergeCell ref="F14:F17"/>
+    <mergeCell ref="A7:A12"/>
+    <mergeCell ref="D21:D26"/>
+    <mergeCell ref="C21:C26"/>
+    <mergeCell ref="A21:A26"/>
+    <mergeCell ref="B14:B17"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="C18:C19"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E0823BC-1B35-46B4-9DFF-9CD2609C03A7}">
+  <dimension ref="A1:J26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.140625" style="19" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" style="16" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" customWidth="1"/>
+    <col min="6" max="6" width="18" customWidth="1"/>
+    <col min="7" max="7" width="18.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" s="22" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A1" s="33" t="s">
+        <v>127</v>
+      </c>
+      <c r="B1" s="37" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="37" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="37" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="37" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="15" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="25" t="s">
+        <v>128</v>
+      </c>
+      <c r="B3" s="35" t="s">
+        <v>90</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="25"/>
+      <c r="B4" s="35" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="A7" s="25" t="s">
+        <v>129</v>
+      </c>
+      <c r="B7" s="35" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" s="1">
+        <v>650000</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="25"/>
+      <c r="B8" s="35" t="s">
+        <v>106</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D8" s="1">
+        <v>1028980</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="120" x14ac:dyDescent="0.25">
+      <c r="A9" s="25"/>
+      <c r="B9" s="35" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D9" s="1">
+        <f>490089+177415</f>
+        <v>667504</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="25"/>
+      <c r="B10" s="35" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10" s="1">
+        <v>1232091</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="38"/>
+    </row>
+    <row r="12" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="B12" s="35" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="15"/>
+    </row>
+    <row r="14" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="15"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="15"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="15"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="15"/>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="15"/>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="25" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="25"/>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="25"/>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="25"/>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="25"/>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="25"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A21:A26"/>
+    <mergeCell ref="A7:A10"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="F7" r:id="rId1" xr:uid="{B83954B4-B6D1-48BF-9B2E-8905E8FFD0A7}"/>
+    <hyperlink ref="G7" r:id="rId2" xr:uid="{957338A5-BC66-49D5-8609-3080023068F3}"/>
+    <hyperlink ref="F9" r:id="rId3" xr:uid="{138926C0-AD4A-4096-9A20-9E03FD133BF5}"/>
+    <hyperlink ref="G9" r:id="rId4" xr:uid="{0E297714-3FE4-4E9F-9F33-B16DA1AFEADA}"/>
+    <hyperlink ref="F10" r:id="rId5" xr:uid="{ABE989B2-0C0E-49D2-AF4B-165CA780079F}"/>
+    <hyperlink ref="G10" r:id="rId6" xr:uid="{60EBE0DE-158D-42FA-AA25-7D402307C060}"/>
+    <hyperlink ref="G8" r:id="rId7" xr:uid="{E8A5F076-70E4-4277-8F21-61AFC17F73FE}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98643D4D-D81F-488C-AE56-A70D10E094CB}">
-  <dimension ref="A1:P39"/>
+  <dimension ref="A1:P43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView topLeftCell="B4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15:G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1116,220 +2010,186 @@
         <v>110</v>
       </c>
     </row>
-    <row r="14" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="B14" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="D14" s="1">
-        <f>1244730+1094458</f>
-        <v>2339188</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="G14" t="s">
-        <v>61</v>
-      </c>
-    </row>
     <row r="15" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
         <v>59</v>
       </c>
       <c r="C15" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="B16" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D16" s="1">
+        <f>1244730+1094458</f>
+        <v>2339188</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="G16" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="B17" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="D15" s="1">
+      <c r="D17" s="1">
         <v>1030836</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="E17" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="F15" s="5" t="s">
+      <c r="F17" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="G15" s="5" t="s">
+      <c r="G17" s="5" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="7" t="s">
+    <row r="18" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C18" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="8" t="s">
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="G16" s="8" t="s">
+      <c r="G18" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="H16" s="8"/>
-      <c r="I16" s="8"/>
-    </row>
-    <row r="17" spans="1:10" s="1" customFormat="1" ht="135" x14ac:dyDescent="0.25">
-      <c r="B17" s="1" t="s">
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
+    </row>
+    <row r="19" spans="1:10" s="1" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+      <c r="B19" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C19" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D19" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="E19" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="F17" s="11" t="s">
+      <c r="F19" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="G17" s="5" t="s">
+      <c r="G19" s="5" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
+    <row r="21" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="B21" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="C21" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D19" s="7">
+      <c r="D21" s="7">
         <v>76995</v>
       </c>
-      <c r="E19" s="7" t="s">
+      <c r="E21" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="F19" s="10" t="s">
+      <c r="F21" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="G19" s="8" t="s">
+      <c r="G21" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="J19" s="1"/>
-    </row>
-    <row r="20" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B20" s="1" t="s">
+      <c r="J21" s="1"/>
+    </row>
+    <row r="22" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="B22" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C22" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D20" s="1">
+      <c r="D22" s="1">
         <v>271570</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="E22" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F20" s="5" t="s">
+      <c r="F22" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="G20" s="5" t="s">
+      <c r="G22" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:10" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A21" s="7"/>
-      <c r="B21" s="7" t="s">
+    <row r="23" spans="1:10" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A23" s="7"/>
+      <c r="B23" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="C23" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D21" s="7">
+      <c r="D23" s="7">
         <v>44456</v>
       </c>
-      <c r="E21" s="7" t="s">
+      <c r="E23" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="F21" s="8" t="s">
+      <c r="F23" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="G21" s="8" t="s">
+      <c r="G23" s="8" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:10" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="7"/>
-      <c r="B22" s="7" t="s">
+    <row r="24" spans="1:10" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" s="7"/>
+      <c r="B24" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="C24" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D22" s="7">
+      <c r="D24" s="7">
         <v>44456</v>
       </c>
-      <c r="E22" s="7" t="s">
+      <c r="E24" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="F22" s="8" t="s">
+      <c r="F24" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="G22" s="8" t="s">
+      <c r="G24" s="8" t="s">
         <v>20</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B23" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D23" s="1">
-        <v>29000</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F23" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="G23" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="J23" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B24" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D24" s="1">
-        <v>29000</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F24" t="s">
-        <v>38</v>
-      </c>
-      <c r="G24" t="s">
-        <v>32</v>
-      </c>
-      <c r="J24" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s">
-        <v>35</v>
+        <v>14</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>34</v>
@@ -1340,40 +2200,42 @@
       <c r="E25" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F25" t="s">
+      <c r="F25" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="G25" t="s">
+      <c r="G25" s="6" t="s">
         <v>32</v>
       </c>
       <c r="J25" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="26" spans="1:10" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="7"/>
-      <c r="B26" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="C26" s="7" t="s">
+    <row r="26" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="B26" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D26" s="7">
+      <c r="D26" s="1">
         <v>29000</v>
       </c>
-      <c r="E26" s="7" t="s">
+      <c r="E26" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F26" s="8" t="s">
+      <c r="F26" t="s">
         <v>38</v>
       </c>
-      <c r="G26" s="8" t="s">
+      <c r="G26" t="s">
         <v>32</v>
+      </c>
+      <c r="J26" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>34</v>
@@ -1394,132 +2256,136 @@
         <v>111</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
+    <row r="28" spans="1:10" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="7"/>
+      <c r="B28" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D28" s="7">
+        <v>29000</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="F28" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="G28" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="B29" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D29" s="1">
+        <v>29000</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F29" t="s">
+        <v>38</v>
+      </c>
+      <c r="G29" t="s">
+        <v>32</v>
+      </c>
+      <c r="J29" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B31" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="C31" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D29" s="1">
+      <c r="D31" s="1">
         <v>43881</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F29" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="G29" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="B30" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D30" s="1">
-        <v>39559</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F30" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="G30" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="B31" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D31" s="1">
-        <v>39560</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>26</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>67</v>
+        <v>30</v>
       </c>
       <c r="G31" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="B32" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>64</v>
       </c>
       <c r="D32" s="1">
-        <v>39561</v>
+        <v>39559</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>26</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G32" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="33" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:7" ht="60" x14ac:dyDescent="0.25">
       <c r="B33" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="D33" s="1">
-        <v>40000</v>
+        <v>39560</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>26</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="G33" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="34" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" ht="60" x14ac:dyDescent="0.25">
       <c r="B34" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="D34" s="1">
-        <v>40000</v>
+        <v>39561</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F34" t="s">
-        <v>72</v>
-      </c>
-      <c r="G34" s="5" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="35" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="F34" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="G34" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B35" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>73</v>
@@ -1530,16 +2396,16 @@
       <c r="E35" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F35" t="s">
+      <c r="F35" s="5" t="s">
         <v>72</v>
       </c>
       <c r="G35" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="36" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B36" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>73</v>
@@ -1553,13 +2419,13 @@
       <c r="F36" t="s">
         <v>72</v>
       </c>
-      <c r="G36" t="s">
+      <c r="G36" s="5" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="37" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B37" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>73</v>
@@ -1579,7 +2445,7 @@
     </row>
     <row r="38" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B38" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>73</v>
@@ -1599,7 +2465,7 @@
     </row>
     <row r="39" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B39" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>73</v>
@@ -1615,6 +2481,66 @@
       </c>
       <c r="G39" t="s">
         <v>71</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B40" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D40" s="1">
+        <v>40000</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F40" t="s">
+        <v>72</v>
+      </c>
+      <c r="G40" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="41" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B41" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D41" s="1">
+        <v>40000</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F41" t="s">
+        <v>72</v>
+      </c>
+      <c r="G41" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="43" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B43" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D43" s="1">
+        <v>36083</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F43" t="s">
+        <v>122</v>
+      </c>
+      <c r="G43" t="s">
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -1622,33 +2548,296 @@
   <hyperlinks>
     <hyperlink ref="F9" r:id="rId1" xr:uid="{ECF4F655-E178-4EE0-89D7-734F17D2F16A}"/>
     <hyperlink ref="F8" r:id="rId2" xr:uid="{1273BF52-00A0-4A9B-9D20-9D822A3E0579}"/>
-    <hyperlink ref="G23" r:id="rId3" xr:uid="{C9981D4E-A240-45B0-B8B5-79F8E1938D29}"/>
-    <hyperlink ref="F23" r:id="rId4" xr:uid="{93E1FBD9-0952-41E8-98C7-20CFAD07CAF1}"/>
-    <hyperlink ref="F29" r:id="rId5" xr:uid="{348392FE-469C-4368-AF97-0DFDFDE1BBC2}"/>
-    <hyperlink ref="F33" r:id="rId6" xr:uid="{5E4F1FBC-90EA-4C55-BF82-59E32CDDC7B1}"/>
+    <hyperlink ref="G25" r:id="rId3" xr:uid="{C9981D4E-A240-45B0-B8B5-79F8E1938D29}"/>
+    <hyperlink ref="F25" r:id="rId4" xr:uid="{93E1FBD9-0952-41E8-98C7-20CFAD07CAF1}"/>
+    <hyperlink ref="F31" r:id="rId5" xr:uid="{348392FE-469C-4368-AF97-0DFDFDE1BBC2}"/>
+    <hyperlink ref="F35" r:id="rId6" xr:uid="{5E4F1FBC-90EA-4C55-BF82-59E32CDDC7B1}"/>
     <hyperlink ref="F6" r:id="rId7" xr:uid="{C2A4BD86-1C88-41DF-AF3B-FDF4185041FA}"/>
     <hyperlink ref="F7" r:id="rId8" xr:uid="{946F0F63-1BAB-498F-A4B3-10A5E0D4B596}"/>
     <hyperlink ref="F10" r:id="rId9" xr:uid="{028A7295-1D4D-440C-ACEC-AF44F0910DFD}"/>
     <hyperlink ref="F12" r:id="rId10" xr:uid="{6472D517-A065-4D22-9800-CA201F182F8B}"/>
-    <hyperlink ref="F14" r:id="rId11" xr:uid="{61F7C871-3E8A-4413-B912-F298F684E6E2}"/>
-    <hyperlink ref="F19" r:id="rId12" xr:uid="{B3E8E859-E9CA-4D4C-ABBC-D2D2ACD33977}"/>
-    <hyperlink ref="F20" r:id="rId13" xr:uid="{B3AA269E-BB22-47F9-B230-CD37F742A4BD}"/>
-    <hyperlink ref="F30" r:id="rId14" xr:uid="{5DBE38BD-976C-4E7B-9259-8CBF010AB9F2}"/>
-    <hyperlink ref="F31" r:id="rId15" xr:uid="{821F5878-37F7-4D33-82CB-063EC715B57D}"/>
-    <hyperlink ref="F32" r:id="rId16" xr:uid="{87E24D2C-01A7-459A-AA07-0E9F5D9BC565}"/>
-    <hyperlink ref="F17" r:id="rId17" xr:uid="{134B2401-7753-4018-9860-CE334DB4FD0C}"/>
-    <hyperlink ref="G34" r:id="rId18" xr:uid="{7F90313D-72F8-47C9-B2EF-7402CCA8A3AB}"/>
+    <hyperlink ref="F16" r:id="rId11" xr:uid="{61F7C871-3E8A-4413-B912-F298F684E6E2}"/>
+    <hyperlink ref="F21" r:id="rId12" xr:uid="{B3E8E859-E9CA-4D4C-ABBC-D2D2ACD33977}"/>
+    <hyperlink ref="F22" r:id="rId13" xr:uid="{B3AA269E-BB22-47F9-B230-CD37F742A4BD}"/>
+    <hyperlink ref="F32" r:id="rId14" xr:uid="{5DBE38BD-976C-4E7B-9259-8CBF010AB9F2}"/>
+    <hyperlink ref="F33" r:id="rId15" xr:uid="{821F5878-37F7-4D33-82CB-063EC715B57D}"/>
+    <hyperlink ref="F34" r:id="rId16" xr:uid="{87E24D2C-01A7-459A-AA07-0E9F5D9BC565}"/>
+    <hyperlink ref="F19" r:id="rId17" xr:uid="{134B2401-7753-4018-9860-CE334DB4FD0C}"/>
+    <hyperlink ref="G36" r:id="rId18" xr:uid="{7F90313D-72F8-47C9-B2EF-7402CCA8A3AB}"/>
     <hyperlink ref="G11" r:id="rId19" xr:uid="{C54A08BF-6753-478C-BCB8-7FBF638238F0}"/>
     <hyperlink ref="G8" r:id="rId20" xr:uid="{D6066E50-6181-45C1-94F2-9CC4AF873BCD}"/>
     <hyperlink ref="G9" r:id="rId21" xr:uid="{9E60432D-C09C-4A05-A397-2E92DF8A13D5}"/>
     <hyperlink ref="G12" r:id="rId22" xr:uid="{C8C2B3BB-7BB3-4C3E-9832-31EC540B4332}"/>
     <hyperlink ref="G13" r:id="rId23" xr:uid="{648F14F6-5F11-4296-A780-A8772A4579F7}"/>
-    <hyperlink ref="G15" r:id="rId24" xr:uid="{F8E7165D-27DE-4CED-B3DE-8AD8C071A2B4}"/>
-    <hyperlink ref="G17" r:id="rId25" xr:uid="{5B1DED33-C4A2-45BF-9F22-F13E8CCDF22F}"/>
-    <hyperlink ref="G20" r:id="rId26" xr:uid="{4F1981B0-7EFB-4F42-A200-A34454FA0B91}"/>
+    <hyperlink ref="G17" r:id="rId24" xr:uid="{F8E7165D-27DE-4CED-B3DE-8AD8C071A2B4}"/>
+    <hyperlink ref="G19" r:id="rId25" xr:uid="{5B1DED33-C4A2-45BF-9F22-F13E8CCDF22F}"/>
+    <hyperlink ref="G22" r:id="rId26" xr:uid="{4F1981B0-7EFB-4F42-A200-A34454FA0B91}"/>
     <hyperlink ref="G6" r:id="rId27" xr:uid="{D46A5282-E6F3-4D01-9D0F-052714C45259}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId28"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC2277AB-6A98-4C33-961A-B79E9F2A4265}">
+  <dimension ref="A1:G30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.140625" style="19" customWidth="1"/>
+    <col min="2" max="2" width="28.42578125" style="17" customWidth="1"/>
+    <col min="3" max="3" width="27" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" customWidth="1"/>
+    <col min="6" max="6" width="18.5703125" customWidth="1"/>
+    <col min="7" max="7" width="18.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="20" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="20" t="s">
+        <v>127</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>133</v>
+      </c>
+      <c r="C1" s="28" t="s">
+        <v>134</v>
+      </c>
+      <c r="D1" s="28"/>
+      <c r="F1" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="G1" s="28"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C2" s="20" t="s">
+        <v>124</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>125</v>
+      </c>
+      <c r="F2" s="20" t="s">
+        <v>124</v>
+      </c>
+      <c r="G2" s="20" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="25" t="s">
+        <v>128</v>
+      </c>
+      <c r="B3" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="C3" t="s">
+        <v>136</v>
+      </c>
+      <c r="D3" t="s">
+        <v>136</v>
+      </c>
+      <c r="F3" t="s">
+        <v>136</v>
+      </c>
+      <c r="G3" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="25"/>
+      <c r="B4" s="21" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="21"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="25" t="s">
+        <v>129</v>
+      </c>
+      <c r="B6" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="F6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G6" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="25"/>
+      <c r="B7" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="F7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G7" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="25"/>
+      <c r="B8" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="F8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G8" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="25"/>
+      <c r="B9" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="F9" t="s">
+        <v>3</v>
+      </c>
+      <c r="G9" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="25"/>
+      <c r="B10" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="F10" t="s">
+        <v>3</v>
+      </c>
+      <c r="G10" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="25" t="s">
+        <v>131</v>
+      </c>
+      <c r="B12" s="21" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="25"/>
+      <c r="B13" s="21" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="25"/>
+      <c r="B14" s="21" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="25"/>
+      <c r="B15" s="21" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="25"/>
+      <c r="B16" s="21" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="27" t="s">
+        <v>132</v>
+      </c>
+      <c r="B18" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" t="s">
+        <v>3</v>
+      </c>
+      <c r="D18" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" s="27"/>
+      <c r="B19" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="C19" t="s">
+        <v>3</v>
+      </c>
+      <c r="D19" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="27"/>
+      <c r="B20" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="C20" t="s">
+        <v>3</v>
+      </c>
+      <c r="D20" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="27"/>
+      <c r="B21" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="C21" t="s">
+        <v>3</v>
+      </c>
+      <c r="D21" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B22" s="21"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B23" s="21"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B24" s="21"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B25" s="21"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B26" s="21"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B27" s="21"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B28" s="21"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B29" s="21"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B30" s="21"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="A6:A10"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A12:A16"/>
+    <mergeCell ref="A18:A21"/>
+    <mergeCell ref="C1:D1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Final list of phenotypes for mutliphenotype MR
</commit_message>
<xml_diff>
--- a/1_data/gwas_summstats/hcm_related_traits_summary.xlsx
+++ b/1_data/gwas_summstats/hcm_related_traits_summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jon Chan\Documents\R Projects\Watkins_Offline\MultiPheno_HCM_MR\1_data\gwas_summstats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F4F8DB9-FD61-427F-94A3-42C5260C10A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F47E9472-F494-4927-BEED-CB98C9286204}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{73FD91AA-0239-4790-95FD-809D24710730}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="197">
   <si>
     <t>TRAIT GROUP</t>
   </si>
@@ -594,6 +594,42 @@
   </si>
   <si>
     <t>Myocardial fibrosis - native T1 time</t>
+  </si>
+  <si>
+    <t>Diastolic function - maxLAVi</t>
+  </si>
+  <si>
+    <t>Diastolic function - Longitudinal PDSR</t>
+  </si>
+  <si>
+    <t>Diastolic function - Radial PDSR</t>
+  </si>
+  <si>
+    <t>Plasma Proteins</t>
+  </si>
+  <si>
+    <t>Plasma Proteins (HCMR)</t>
+  </si>
+  <si>
+    <t>Troponin T</t>
+  </si>
+  <si>
+    <t>HCMR</t>
+  </si>
+  <si>
+    <t>C1CP</t>
+  </si>
+  <si>
+    <t>In-house GWAS (without UKB controls from Harper 2021)</t>
+  </si>
+  <si>
+    <t>In-house GWAS of HCMR cases</t>
+  </si>
+  <si>
+    <t>Myocardial fibrosis - LGE</t>
+  </si>
+  <si>
+    <t>Myocardial fibrosis - ECVFwhole</t>
   </si>
 </sst>
 </file>
@@ -1160,7 +1196,7 @@
   <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18:B19"/>
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1437,7 +1473,7 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="25" t="s">
-        <v>160</v>
+        <v>188</v>
       </c>
       <c r="B21" s="16" t="s">
         <v>156</v>
@@ -1532,17 +1568,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E0823BC-1B35-46B4-9DFF-9CD2609C03A7}">
-  <dimension ref="A1:J26"/>
+  <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.140625" style="19" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" style="16" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" style="35" customWidth="1"/>
     <col min="3" max="3" width="18.5703125" customWidth="1"/>
+    <col min="5" max="5" width="21.140625" style="1" customWidth="1"/>
     <col min="6" max="6" width="18" customWidth="1"/>
     <col min="7" max="7" width="18.28515625" customWidth="1"/>
   </cols>
@@ -1595,13 +1632,12 @@
         <v>126</v>
       </c>
       <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
       <c r="F4" s="5"/>
       <c r="G4" s="5" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="25" t="s">
         <v>129</v>
       </c>
@@ -1624,7 +1660,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="25"/>
       <c r="B8" s="35" t="s">
         <v>106</v>
@@ -1645,7 +1681,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="120" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="25"/>
       <c r="B9" s="35" t="s">
         <v>48</v>
@@ -1692,56 +1728,258 @@
       <c r="A11" s="38"/>
     </row>
     <row r="12" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="15" t="s">
+      <c r="A12" s="27" t="s">
         <v>157</v>
       </c>
       <c r="B12" s="35" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="15"/>
-    </row>
-    <row r="14" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="15"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="15"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="15"/>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="15"/>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="15"/>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="25" t="s">
+      <c r="C12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="1">
+        <v>43881</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="27"/>
+      <c r="B13" s="35" t="s">
+        <v>196</v>
+      </c>
+      <c r="C13" s="22" t="s">
+        <v>194</v>
+      </c>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="F13" s="5"/>
+    </row>
+    <row r="14" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="27"/>
+      <c r="B14" s="35" t="s">
+        <v>195</v>
+      </c>
+      <c r="C14" s="35" t="s">
+        <v>194</v>
+      </c>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="F14" s="5"/>
+    </row>
+    <row r="15" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="27"/>
+      <c r="B15" s="35" t="s">
+        <v>185</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D15" s="1">
+        <v>39561</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="G15" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="27"/>
+      <c r="B16" s="35" t="s">
+        <v>186</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D16" s="1">
+        <v>39559</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="G16" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="27"/>
+      <c r="B17" s="35" t="s">
+        <v>187</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D17" s="1">
+        <v>39560</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="G17" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="15"/>
+    </row>
+    <row r="19" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="25" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B19" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C19" s="36" t="s">
+        <v>193</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="25"/>
+      <c r="B20" s="16" t="s">
+        <v>164</v>
+      </c>
+      <c r="C20" s="36"/>
+      <c r="E20" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="25"/>
+      <c r="B21" s="16" t="s">
+        <v>162</v>
+      </c>
+      <c r="C21" s="36"/>
+      <c r="E21" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="25"/>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B22" s="16" t="s">
+        <v>159</v>
+      </c>
+      <c r="C22" s="36"/>
+      <c r="E22" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="25"/>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B23" s="16" t="s">
+        <v>158</v>
+      </c>
+      <c r="C23" s="36"/>
+      <c r="E23" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="25"/>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="25"/>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" s="25"/>
+      <c r="B24" s="16" t="s">
+        <v>161</v>
+      </c>
+      <c r="C24" s="36"/>
+      <c r="E24" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="38"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="38" t="s">
+        <v>189</v>
+      </c>
+      <c r="B26" s="35" t="s">
+        <v>156</v>
+      </c>
+      <c r="C26" s="36" t="s">
+        <v>194</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="38"/>
+      <c r="B27" s="35" t="s">
+        <v>190</v>
+      </c>
+      <c r="C27" s="36"/>
+      <c r="E27" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="38"/>
+      <c r="B28" s="16" t="s">
+        <v>159</v>
+      </c>
+      <c r="C28" s="36"/>
+      <c r="E28" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B29" s="16" t="s">
+        <v>158</v>
+      </c>
+      <c r="C29" s="36"/>
+      <c r="E29" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B30" s="16" t="s">
+        <v>161</v>
+      </c>
+      <c r="C30" s="36"/>
+      <c r="E30" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B31" s="35" t="s">
+        <v>192</v>
+      </c>
+      <c r="C31" s="36"/>
+      <c r="E31" s="1" t="s">
+        <v>191</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="6">
+    <mergeCell ref="C19:C24"/>
+    <mergeCell ref="C26:C31"/>
+    <mergeCell ref="A12:A17"/>
     <mergeCell ref="A3:A4"/>
-    <mergeCell ref="A21:A26"/>
     <mergeCell ref="A7:A10"/>
+    <mergeCell ref="A19:A24"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F7" r:id="rId1" xr:uid="{B83954B4-B6D1-48BF-9B2E-8905E8FFD0A7}"/>
@@ -1751,6 +1989,10 @@
     <hyperlink ref="F10" r:id="rId5" xr:uid="{ABE989B2-0C0E-49D2-AF4B-165CA780079F}"/>
     <hyperlink ref="G10" r:id="rId6" xr:uid="{60EBE0DE-158D-42FA-AA25-7D402307C060}"/>
     <hyperlink ref="G8" r:id="rId7" xr:uid="{E8A5F076-70E4-4277-8F21-61AFC17F73FE}"/>
+    <hyperlink ref="F12" r:id="rId8" xr:uid="{EEB667E5-44BE-44E4-B491-53F3A8E8504F}"/>
+    <hyperlink ref="F16" r:id="rId9" xr:uid="{28212A0C-B9FD-46E8-B44E-D8ACF717F21F}"/>
+    <hyperlink ref="F17" r:id="rId10" xr:uid="{97167BEB-91A0-4AAE-A67E-6AF177E3CDC0}"/>
+    <hyperlink ref="F15" r:id="rId11" xr:uid="{5BC3D297-B9F4-4C2E-AF0F-00B940C4F351}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1760,8 +2002,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98643D4D-D81F-488C-AE56-A70D10E094CB}">
   <dimension ref="A1:P43"/>
   <sheetViews>
-    <sheetView topLeftCell="B4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15:G15"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>